<commit_message>
Possibilité de sauvegarder la BDD sur un fichier Excel via le module "openpyxl".
</commit_message>
<xml_diff>
--- a/src/streams/Tableur.xlsx
+++ b/src/streams/Tableur.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Authors" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t xml:space="preserve">lastname</t>
   </si>
@@ -155,16 +155,16 @@
     <t xml:space="preserve">Zadig</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-09-05 15:31:22.111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-09-05 15:31:22.333555</t>
+    <t xml:space="preserve">Flammarion</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
     <t xml:space="preserve">Durance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coiffard</t>
   </si>
 </sst>
 </file>
@@ -289,7 +289,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.93"/>
@@ -378,7 +378,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.23"/>
@@ -533,8 +533,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,8 +575,8 @@
       <c r="D2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>43</v>
+      <c r="E2" s="5" t="n">
+        <v>44809.6475347222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,13 +587,13 @@
         <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>44</v>
+      <c r="E3" s="5" t="n">
+        <v>44809.6466666667</v>
       </c>
     </row>
   </sheetData>
@@ -612,17 +612,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>3</v>
@@ -633,12 +633,23 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>